<commit_message>
Adding test cases and updating Gnatt Chart
</commit_message>
<xml_diff>
--- a/DOOOM_Gantt_Chart.xlsx
+++ b/DOOOM_Gantt_Chart.xlsx
@@ -458,6 +458,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -467,20 +481,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,10 +784,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A28" sqref="A28"/>
-      <selection pane="topRight" activeCell="BW62" sqref="BW62"/>
+      <selection pane="topRight" activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,89 +818,89 @@
       <c r="B3" s="22"/>
     </row>
     <row r="4" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="31" t="s">
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32"/>
-      <c r="X4" s="32"/>
-      <c r="Y4" s="32"/>
-      <c r="Z4" s="32"/>
-      <c r="AA4" s="32"/>
-      <c r="AB4" s="32"/>
-      <c r="AC4" s="32"/>
-      <c r="AD4" s="32"/>
-      <c r="AE4" s="32"/>
-      <c r="AF4" s="32"/>
-      <c r="AG4" s="32"/>
-      <c r="AH4" s="32"/>
-      <c r="AI4" s="32"/>
-      <c r="AJ4" s="32"/>
-      <c r="AK4" s="32"/>
-      <c r="AL4" s="33"/>
-      <c r="AM4" s="31" t="s">
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="33"/>
+      <c r="X4" s="33"/>
+      <c r="Y4" s="33"/>
+      <c r="Z4" s="33"/>
+      <c r="AA4" s="33"/>
+      <c r="AB4" s="33"/>
+      <c r="AC4" s="33"/>
+      <c r="AD4" s="33"/>
+      <c r="AE4" s="33"/>
+      <c r="AF4" s="33"/>
+      <c r="AG4" s="33"/>
+      <c r="AH4" s="33"/>
+      <c r="AI4" s="33"/>
+      <c r="AJ4" s="33"/>
+      <c r="AK4" s="33"/>
+      <c r="AL4" s="34"/>
+      <c r="AM4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="AN4" s="32"/>
-      <c r="AO4" s="32"/>
-      <c r="AP4" s="32"/>
-      <c r="AQ4" s="32"/>
-      <c r="AR4" s="32"/>
-      <c r="AS4" s="32"/>
-      <c r="AT4" s="32"/>
-      <c r="AU4" s="32"/>
-      <c r="AV4" s="32"/>
-      <c r="AW4" s="32"/>
-      <c r="AX4" s="32"/>
-      <c r="AY4" s="32"/>
-      <c r="AZ4" s="32"/>
-      <c r="BA4" s="32"/>
-      <c r="BB4" s="32"/>
-      <c r="BC4" s="32"/>
-      <c r="BD4" s="32"/>
-      <c r="BE4" s="32"/>
-      <c r="BF4" s="32"/>
-      <c r="BG4" s="32" t="s">
+      <c r="AN4" s="33"/>
+      <c r="AO4" s="33"/>
+      <c r="AP4" s="33"/>
+      <c r="AQ4" s="33"/>
+      <c r="AR4" s="33"/>
+      <c r="AS4" s="33"/>
+      <c r="AT4" s="33"/>
+      <c r="AU4" s="33"/>
+      <c r="AV4" s="33"/>
+      <c r="AW4" s="33"/>
+      <c r="AX4" s="33"/>
+      <c r="AY4" s="33"/>
+      <c r="AZ4" s="33"/>
+      <c r="BA4" s="33"/>
+      <c r="BB4" s="33"/>
+      <c r="BC4" s="33"/>
+      <c r="BD4" s="33"/>
+      <c r="BE4" s="33"/>
+      <c r="BF4" s="33"/>
+      <c r="BG4" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="BH4" s="32"/>
-      <c r="BI4" s="32"/>
-      <c r="BJ4" s="32"/>
-      <c r="BK4" s="32"/>
-      <c r="BL4" s="32"/>
-      <c r="BM4" s="32"/>
-      <c r="BN4" s="32"/>
-      <c r="BO4" s="32"/>
-      <c r="BP4" s="32"/>
-      <c r="BQ4" s="32"/>
-      <c r="BR4" s="32"/>
-      <c r="BS4" s="32"/>
-      <c r="BT4" s="32"/>
-      <c r="BU4" s="32"/>
-      <c r="BV4" s="32"/>
-      <c r="BW4" s="32"/>
-      <c r="BX4" s="32"/>
-      <c r="BY4" s="32"/>
-      <c r="BZ4" s="33"/>
+      <c r="BH4" s="33"/>
+      <c r="BI4" s="33"/>
+      <c r="BJ4" s="33"/>
+      <c r="BK4" s="33"/>
+      <c r="BL4" s="33"/>
+      <c r="BM4" s="33"/>
+      <c r="BN4" s="33"/>
+      <c r="BO4" s="33"/>
+      <c r="BP4" s="33"/>
+      <c r="BQ4" s="33"/>
+      <c r="BR4" s="33"/>
+      <c r="BS4" s="33"/>
+      <c r="BT4" s="33"/>
+      <c r="BU4" s="33"/>
+      <c r="BV4" s="33"/>
+      <c r="BW4" s="33"/>
+      <c r="BX4" s="33"/>
+      <c r="BY4" s="33"/>
+      <c r="BZ4" s="34"/>
     </row>
     <row r="5" spans="1:78" x14ac:dyDescent="0.25">
       <c r="D5">
@@ -1122,10 +1122,10 @@
       <c r="BX5" s="3">
         <v>17</v>
       </c>
-      <c r="BY5" s="36">
+      <c r="BY5" s="30">
         <v>18</v>
       </c>
-      <c r="BZ5" s="37">
+      <c r="BZ5" s="31">
         <v>19</v>
       </c>
     </row>
@@ -1137,111 +1137,111 @@
       <c r="C6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="31" t="s">
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="31" t="s">
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="31" t="s">
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="34"/>
+      <c r="S6" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="T6" s="32"/>
-      <c r="U6" s="32"/>
-      <c r="V6" s="32"/>
-      <c r="W6" s="33"/>
-      <c r="X6" s="31" t="s">
+      <c r="T6" s="33"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="33"/>
+      <c r="W6" s="34"/>
+      <c r="X6" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="Y6" s="32"/>
-      <c r="Z6" s="32"/>
-      <c r="AA6" s="32"/>
-      <c r="AB6" s="33"/>
-      <c r="AC6" s="31" t="s">
+      <c r="Y6" s="33"/>
+      <c r="Z6" s="33"/>
+      <c r="AA6" s="33"/>
+      <c r="AB6" s="34"/>
+      <c r="AC6" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="AD6" s="32"/>
-      <c r="AE6" s="32"/>
-      <c r="AF6" s="32"/>
-      <c r="AG6" s="33"/>
-      <c r="AH6" s="31" t="s">
+      <c r="AD6" s="33"/>
+      <c r="AE6" s="33"/>
+      <c r="AF6" s="33"/>
+      <c r="AG6" s="34"/>
+      <c r="AH6" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="AI6" s="32"/>
-      <c r="AJ6" s="32"/>
-      <c r="AK6" s="32"/>
-      <c r="AL6" s="33"/>
-      <c r="AM6" s="31" t="s">
+      <c r="AI6" s="33"/>
+      <c r="AJ6" s="33"/>
+      <c r="AK6" s="33"/>
+      <c r="AL6" s="34"/>
+      <c r="AM6" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="AN6" s="32"/>
-      <c r="AO6" s="32"/>
-      <c r="AP6" s="32"/>
-      <c r="AQ6" s="33"/>
-      <c r="AR6" s="31" t="s">
+      <c r="AN6" s="33"/>
+      <c r="AO6" s="33"/>
+      <c r="AP6" s="33"/>
+      <c r="AQ6" s="34"/>
+      <c r="AR6" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="AS6" s="32"/>
-      <c r="AT6" s="32"/>
-      <c r="AU6" s="32"/>
-      <c r="AV6" s="33"/>
-      <c r="AW6" s="31" t="s">
+      <c r="AS6" s="33"/>
+      <c r="AT6" s="33"/>
+      <c r="AU6" s="33"/>
+      <c r="AV6" s="34"/>
+      <c r="AW6" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="AX6" s="32"/>
-      <c r="AY6" s="32"/>
-      <c r="AZ6" s="32"/>
-      <c r="BA6" s="33"/>
-      <c r="BB6" s="31" t="s">
+      <c r="AX6" s="33"/>
+      <c r="AY6" s="33"/>
+      <c r="AZ6" s="33"/>
+      <c r="BA6" s="34"/>
+      <c r="BB6" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="BC6" s="32"/>
-      <c r="BD6" s="32"/>
-      <c r="BE6" s="32"/>
-      <c r="BF6" s="32"/>
-      <c r="BG6" s="31" t="s">
+      <c r="BC6" s="33"/>
+      <c r="BD6" s="33"/>
+      <c r="BE6" s="33"/>
+      <c r="BF6" s="33"/>
+      <c r="BG6" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="BH6" s="32"/>
-      <c r="BI6" s="32"/>
-      <c r="BJ6" s="32"/>
-      <c r="BK6" s="33"/>
-      <c r="BL6" s="31" t="s">
+      <c r="BH6" s="33"/>
+      <c r="BI6" s="33"/>
+      <c r="BJ6" s="33"/>
+      <c r="BK6" s="34"/>
+      <c r="BL6" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="BM6" s="32"/>
-      <c r="BN6" s="32"/>
-      <c r="BO6" s="32"/>
-      <c r="BP6" s="33"/>
-      <c r="BQ6" s="31" t="s">
+      <c r="BM6" s="33"/>
+      <c r="BN6" s="33"/>
+      <c r="BO6" s="33"/>
+      <c r="BP6" s="34"/>
+      <c r="BQ6" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="BR6" s="32"/>
-      <c r="BS6" s="32"/>
-      <c r="BT6" s="32"/>
-      <c r="BU6" s="33"/>
-      <c r="BV6" s="31" t="s">
+      <c r="BR6" s="33"/>
+      <c r="BS6" s="33"/>
+      <c r="BT6" s="33"/>
+      <c r="BU6" s="34"/>
+      <c r="BV6" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="BW6" s="32"/>
-      <c r="BX6" s="32"/>
-      <c r="BY6" s="32"/>
-      <c r="BZ6" s="33"/>
+      <c r="BW6" s="33"/>
+      <c r="BX6" s="33"/>
+      <c r="BY6" s="33"/>
+      <c r="BZ6" s="34"/>
     </row>
     <row r="7" spans="1:78" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
@@ -1306,26 +1306,26 @@
       <c r="BD7" s="10"/>
       <c r="BE7" s="10"/>
       <c r="BF7" s="10"/>
-      <c r="BG7" s="34"/>
-      <c r="BH7" s="34"/>
-      <c r="BI7" s="34"/>
-      <c r="BJ7" s="34"/>
-      <c r="BK7" s="34"/>
-      <c r="BL7" s="34"/>
-      <c r="BM7" s="34"/>
-      <c r="BN7" s="34"/>
-      <c r="BO7" s="34"/>
-      <c r="BP7" s="34"/>
-      <c r="BQ7" s="34"/>
-      <c r="BR7" s="34"/>
-      <c r="BS7" s="34"/>
-      <c r="BT7" s="34"/>
-      <c r="BU7" s="34"/>
-      <c r="BV7" s="34"/>
-      <c r="BW7" s="34"/>
-      <c r="BX7" s="34"/>
-      <c r="BY7" s="34"/>
-      <c r="BZ7" s="35"/>
+      <c r="BG7" s="28"/>
+      <c r="BH7" s="28"/>
+      <c r="BI7" s="28"/>
+      <c r="BJ7" s="28"/>
+      <c r="BK7" s="28"/>
+      <c r="BL7" s="28"/>
+      <c r="BM7" s="28"/>
+      <c r="BN7" s="28"/>
+      <c r="BO7" s="28"/>
+      <c r="BP7" s="28"/>
+      <c r="BQ7" s="28"/>
+      <c r="BR7" s="28"/>
+      <c r="BS7" s="28"/>
+      <c r="BT7" s="28"/>
+      <c r="BU7" s="28"/>
+      <c r="BV7" s="28"/>
+      <c r="BW7" s="28"/>
+      <c r="BX7" s="28"/>
+      <c r="BY7" s="28"/>
+      <c r="BZ7" s="29"/>
     </row>
     <row r="8" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -54200,7 +54200,7 @@
       <c r="BJ54" s="3"/>
       <c r="BK54" s="25"/>
       <c r="BL54" s="25"/>
-      <c r="BM54" s="38"/>
+      <c r="BM54" s="32"/>
       <c r="BN54" s="3"/>
       <c r="BO54" s="23"/>
       <c r="BP54" s="3"/>
@@ -54475,7 +54475,7 @@
     </row>
     <row r="58" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B58">
         <v>6.9</v>
@@ -56717,11 +56717,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="BG4:BZ4"/>
-    <mergeCell ref="BG6:BK6"/>
-    <mergeCell ref="BL6:BP6"/>
-    <mergeCell ref="BQ6:BU6"/>
-    <mergeCell ref="BV6:BZ6"/>
     <mergeCell ref="D4:R4"/>
     <mergeCell ref="S4:AL4"/>
     <mergeCell ref="AM4:BF4"/>
@@ -56736,6 +56731,11 @@
     <mergeCell ref="N6:R6"/>
     <mergeCell ref="S6:W6"/>
     <mergeCell ref="X6:AB6"/>
+    <mergeCell ref="BG4:BZ4"/>
+    <mergeCell ref="BG6:BK6"/>
+    <mergeCell ref="BL6:BP6"/>
+    <mergeCell ref="BQ6:BU6"/>
+    <mergeCell ref="BV6:BZ6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>